<commit_message>
Add simple MVVM, command buffering.
Command buffering ensures that all commands in a set of commands (like
"dimmer 58 at 25 go") get sent in one packet, instead of in several
packets, to ensure that they arrive in order.
</commit_message>
<xml_diff>
--- a/RFU Keymap.xlsx
+++ b/RFU Keymap.xlsx
@@ -5,11 +5,11 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/ce7ea6ba70daaabb/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Matthew\GitHub\rfu\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="3795" windowHeight="4125"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="3795" windowHeight="2775"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -466,7 +466,7 @@
   <dimension ref="A1:D41"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C41" sqref="C41"/>
+      <selection activeCell="A31" sqref="A31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>